<commit_message>
feat: Highlight platform in dependency diagram when clicking grid row
When clicking a document type in the grid, the platform from that row
is now highlighted with a yellow background in the dependency diagram modal.
Also fixed case sensitivity issue merging duplicate "Cedula de identidad" entries.
</commit_message>
<xml_diff>
--- a/resources/portals.xlsx
+++ b/resources/portals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tecnova\OneDrive\Mine\document-types-dependency\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tecnova\OneDrive\Mine\dependency-document-types\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D9E104-3F64-4FC9-83B1-076366A55ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4093A617-08B6-464B-9F0E-3B5993A5F6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DC58811-3100-4723-8A47-51BC9F49FBED}"/>
   </bookViews>
@@ -1246,9 +1246,6 @@
     <t>Recibo de conformidad</t>
   </si>
   <si>
-    <t>Cedula de identidad</t>
-  </si>
-  <si>
     <t>Poliza</t>
   </si>
   <si>
@@ -1304,6 +1301,9 @@
   </si>
   <si>
     <t>NO, a menos que el liquidador los solicite, entonces el formulario enviado al cliente obligara a subirlo LAGL.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voucher alcotest </t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1787,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E250" sqref="E250"/>
+      <selection pane="topRight" activeCell="F254" sqref="F254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
@@ -3929,19 +3929,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="3" t="s">
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="D155" t="s">
         <v>27</v>
       </c>
-      <c r="E155" t="s">
-        <v>202</v>
+      <c r="E155" s="8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -3959,7 +3959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>129</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>129</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>129</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>129</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="161" spans="1:7" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>129</v>
       </c>
@@ -4821,12 +4821,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
         <v>181</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="D220" t="s">
         <v>25</v>
@@ -4838,15 +4838,15 @@
         <v>9</v>
       </c>
       <c r="G220" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
     </row>
     <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C221" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C221" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D221" t="s">
         <v>12</v>
@@ -4854,10 +4854,10 @@
     </row>
     <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C222" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D222" t="s">
         <v>27</v>
@@ -4868,10 +4868,10 @@
     </row>
     <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C223" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D223" t="s">
         <v>86</v>
@@ -4882,10 +4882,10 @@
     </row>
     <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C224" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="C224" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="D224" t="s">
         <v>77</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B225" s="7" t="s">
         <v>125</v>
@@ -4911,10 +4911,10 @@
     </row>
     <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D226" t="s">
         <v>60</v>
@@ -4925,21 +4925,21 @@
     </row>
     <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C227" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D227" t="s">
         <v>186</v>
-      </c>
-      <c r="C227" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D227" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>20</v>
@@ -4950,10 +4950,10 @@
     </row>
     <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>20</v>
@@ -4964,10 +4964,10 @@
     </row>
     <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>20</v>
@@ -4978,7 +4978,7 @@
     </row>
     <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B231" s="7">
         <v>1</v>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B232" s="7">
         <v>2</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B233" s="7">
         <v>4</v>
@@ -5020,7 +5020,7 @@
     </row>
     <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B234" s="7">
         <v>5</v>
@@ -5034,7 +5034,7 @@
     </row>
     <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B235" s="7">
         <v>82</v>
@@ -5048,10 +5048,10 @@
     </row>
     <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D236" s="5" t="s">
         <v>20</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D237" s="5" t="s">
         <v>20</v>
@@ -5076,10 +5076,10 @@
     </row>
     <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>20</v>
@@ -5107,7 +5107,7 @@
         <v>10</v>
       </c>
       <c r="C240" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D240" t="s">
         <v>12</v>
@@ -5121,7 +5121,7 @@
         <v>7</v>
       </c>
       <c r="C241" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D241" t="s">
         <v>7</v>
@@ -5135,7 +5135,7 @@
         <v>7</v>
       </c>
       <c r="C242" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D242" t="s">
         <v>7</v>
@@ -5149,7 +5149,7 @@
         <v>7</v>
       </c>
       <c r="C243" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D243" t="s">
         <v>7</v>
@@ -5163,7 +5163,7 @@
         <v>7</v>
       </c>
       <c r="C244" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D244" t="s">
         <v>7</v>
@@ -5177,7 +5177,7 @@
         <v>7</v>
       </c>
       <c r="C245" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D245" t="s">
         <v>7</v>
@@ -5191,7 +5191,7 @@
         <v>7</v>
       </c>
       <c r="C246" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D246" t="s">
         <v>7</v>
@@ -5205,7 +5205,7 @@
         <v>7</v>
       </c>
       <c r="C247" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D247" t="s">
         <v>7</v>
@@ -5219,7 +5219,7 @@
         <v>7</v>
       </c>
       <c r="C248" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D248" t="s">
         <v>7</v>
@@ -5246,7 +5246,7 @@
   <autoFilter ref="A1:G249" xr:uid="{030E9699-145C-4EC8-B54C-AAF5E31C4F71}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Voucher alcotest"/>
+        <filter val="Cedula de Identidad"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
chore: update render.yaml and modify portals.xlsx
- Ensured consistency in render.yaml by maintaining the Python version.
- Updated portals.xlsx with changes to the binary file.
</commit_message>
<xml_diff>
--- a/resources/portals.xlsx
+++ b/resources/portals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tecnova\OneDrive\Mine\dependency-document-types\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32A8BB2-4773-4FE1-8249-A21E668B6D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E31F4E-61DA-4BD1-9B4A-4D29AF8D49BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DC58811-3100-4723-8A47-51BC9F49FBED}"/>
   </bookViews>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="282">
   <si>
     <t>ItemType(AS IS)</t>
   </si>
@@ -6012,6 +6012,9 @@
       <c r="M160" t="s">
         <v>209</v>
       </c>
+      <c r="O160" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">

</xml_diff>